<commit_message>
bug in slicing assumption set
</commit_message>
<xml_diff>
--- a/examples/04_two_state_disability/portfolio/portfolio_small.xlsx
+++ b/examples/04_two_state_disability/portfolio/portfolio_small.xlsx
@@ -105,10 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -415,7 +414,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,7 +425,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="A3:L3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -507,8 +506,8 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="2">
-        <v>44562</v>
+      <c r="L2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12">

</xml_diff>